<commit_message>
soap version with robocorp
</commit_message>
<xml_diff>
--- a/output/articles-brexit.xlsx
+++ b/output/articles-brexit.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>title</t>
   </si>
@@ -116,18 +116,6 @@
   </si>
   <si>
     <t xml:space="preserve"> Britain’s Conservatives suffer historic losses in elections as Labor edges closer to power.jpeg</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Former U.K. leader Liz Truss blames others for her brief, chaotic tenure — and she endorses Trump </t>
-  </si>
-  <si>
-    <t>Liz Truss sparked mayhem on the financial markets and turmoil within her Conservative Party during her 49 days as Britain’s prime minister.</t>
-  </si>
-  <si>
-    <t>04/16/2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Former U.K. leader Liz Truss blames others for her brief, chaotic tenure — and she endorses Trump.jpeg</t>
   </si>
 </sst>
 </file>
@@ -459,7 +447,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -625,26 +613,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
-      <c r="A9" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9" t="b">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>